<commit_message>
added prompts for username and passwords for HX and vCenter
</commit_message>
<xml_diff>
--- a/hx_vcenter_register_input.xlsx
+++ b/hx_vcenter_register_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michzimm/projects/hx_vcenter_register/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1973AB7C-5FA6-AE45-9B75-516C54A24249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B06809-49CE-6F48-AB2C-D4BE7889D0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="1600" windowWidth="28800" windowHeight="17500" xr2:uid="{8BD6B14D-75F5-5845-9EE5-BE45D31404F9}"/>
+    <workbookView xWindow="2700" yWindow="1580" windowWidth="28800" windowHeight="17500" xr2:uid="{8BD6B14D-75F5-5845-9EE5-BE45D31404F9}"/>
   </bookViews>
   <sheets>
     <sheet name="hx_cluster_info" sheetId="1" r:id="rId1"/>
@@ -35,51 +35,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>HyperFlex_FQDN/IP</t>
-  </si>
-  <si>
-    <t>HyperFlex_User</t>
-  </si>
-  <si>
-    <t>HyperFlex_Password</t>
   </si>
   <si>
     <t>vCenter_FQDN/IP</t>
   </si>
   <si>
-    <t>vCenter_User</t>
-  </si>
-  <si>
-    <t>vCenter_Password</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>administrator@vsphere.local</t>
-  </si>
-  <si>
-    <t>vCenter_Datacenter_Name</t>
-  </si>
-  <si>
-    <t>ESXi_Cluster_Name</t>
-  </si>
-  <si>
-    <t>&lt;vcenter_password&gt;</t>
-  </si>
-  <si>
-    <t>&lt;vcenter_datacenter&gt;</t>
-  </si>
-  <si>
-    <t>&lt;vcenter_esxi_cluster_name&gt;</t>
-  </si>
-  <si>
     <t>&lt;vcenter_fqdn/ip&gt;</t>
-  </si>
-  <si>
-    <t>&lt;hx_password&gt;</t>
   </si>
   <si>
     <t>&lt;hx_fqdn/ip&gt;</t>
@@ -89,18 +53,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,19 +92,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,107 +414,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D302E8E-351D-2145-8F6F-50BDAD8F04EE}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C1" sqref="C1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" customWidth="1"/>
-    <col min="7" max="7" width="32.5" customWidth="1"/>
-    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{6A88B1B8-042E-7D45-96E6-4875AAAF7836}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{D371157B-F299-D541-A1E5-B8C379055E15}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>